<commit_message>
added info for turning off hobs observations via pest (not via hobs creation). can turn off GWLE or hobs.
</commit_message>
<xml_diff>
--- a/scripts/HOB_Creation/WellDetails_20240911.xlsx
+++ b/scripts/HOB_Creation/WellDetails_20240911.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GSP\sv\model\update_2024\scripts\HOB_Creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1C97C2-B538-464E-A69E-C74BECE90041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF9B386-6D37-40F8-B9F3-2C5DBAF19475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C36B50A-405C-4BA3-B301-F0A1B218D0FF}"/>
   </bookViews>
@@ -3791,12 +3791,6 @@
     <t>Suggest Inclusion in future update?</t>
   </si>
   <si>
-    <t>HOBS zero weight</t>
-  </si>
-  <si>
-    <t>ALL GWLE zero weight</t>
-  </si>
-  <si>
     <t>GWLE_major_off</t>
   </si>
   <si>
@@ -3840,6 +3834,12 @@
   </si>
   <si>
     <t>Bay</t>
+  </si>
+  <si>
+    <t>ALL_GWLE_zero_weight</t>
+  </si>
+  <si>
+    <t>HOBS_zero_weight</t>
   </si>
 </sst>
 </file>
@@ -4790,10 +4790,10 @@
   <dimension ref="A1:BK261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AP3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BB40" sqref="BB40"/>
+      <selection pane="bottomRight" activeCell="BC26" sqref="BC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5001,7 +5001,7 @@
         <v>996</v>
       </c>
       <c r="BA1" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="BB1" s="2" t="s">
         <v>997</v>
@@ -5013,25 +5013,25 @@
         <v>1223</v>
       </c>
       <c r="BE1" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="BG1" s="2" t="s">
         <v>1237</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>1238</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>1239</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>1240</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>1241</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>1242</v>
-      </c>
-      <c r="BK1" s="2" t="s">
-        <v>1243</v>
       </c>
     </row>
     <row r="2" spans="1:63" hidden="1" x14ac:dyDescent="0.25">
@@ -5145,7 +5145,7 @@
         <v>30</v>
       </c>
       <c r="BA2" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB2">
         <v>13970</v>
@@ -5274,7 +5274,7 @@
         <v>42</v>
       </c>
       <c r="BA3" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB3">
         <v>6842</v>
@@ -5403,7 +5403,7 @@
         <v>50</v>
       </c>
       <c r="BA4" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB4">
         <v>13310</v>
@@ -5532,7 +5532,7 @@
         <v>69</v>
       </c>
       <c r="BA5" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB5">
         <v>12734</v>
@@ -5661,7 +5661,7 @@
         <v>54</v>
       </c>
       <c r="BA6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB6">
         <v>14249</v>
@@ -5790,7 +5790,7 @@
         <v>30</v>
       </c>
       <c r="BA7" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB7">
         <v>14990</v>
@@ -5898,7 +5898,7 @@
         <v>46</v>
       </c>
       <c r="BA8" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB8">
         <v>7101</v>
@@ -6027,7 +6027,7 @@
         <v>50</v>
       </c>
       <c r="BA9" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB9">
         <v>13480</v>
@@ -6126,7 +6126,7 @@
         <v>5</v>
       </c>
       <c r="BA10" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB10">
         <v>2470</v>
@@ -6255,7 +6255,7 @@
         <v>6</v>
       </c>
       <c r="BA11" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB11">
         <v>2471</v>
@@ -6366,7 +6366,7 @@
         <v>33</v>
       </c>
       <c r="BA12" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB12">
         <v>373</v>
@@ -6477,7 +6477,7 @@
         <v>33</v>
       </c>
       <c r="BA13" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB13">
         <v>373</v>
@@ -6588,7 +6588,7 @@
         <v>33</v>
       </c>
       <c r="BA14" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB14">
         <v>458</v>
@@ -6699,7 +6699,7 @@
         <v>33</v>
       </c>
       <c r="BA15" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB15">
         <v>458</v>
@@ -6810,7 +6810,7 @@
         <v>28</v>
       </c>
       <c r="BA16" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB16">
         <v>623</v>
@@ -6942,7 +6942,7 @@
         <v>27</v>
       </c>
       <c r="BA17" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB17">
         <v>707</v>
@@ -7053,7 +7053,7 @@
         <v>26</v>
       </c>
       <c r="BA18" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB18">
         <v>1301</v>
@@ -7191,7 +7191,7 @@
         <v>28</v>
       </c>
       <c r="BA19" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB19">
         <v>1303</v>
@@ -7323,7 +7323,7 @@
         <v>30</v>
       </c>
       <c r="BA20" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB20">
         <v>880</v>
@@ -7431,7 +7431,7 @@
         <v>33</v>
       </c>
       <c r="BA21" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB21">
         <v>3518</v>
@@ -7542,7 +7542,7 @@
         <v>29</v>
       </c>
       <c r="BA22" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB22">
         <v>964</v>
@@ -7653,7 +7653,7 @@
         <v>33</v>
       </c>
       <c r="BA23" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB23">
         <v>1138</v>
@@ -7782,7 +7782,7 @@
         <v>28</v>
       </c>
       <c r="BA24" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB24">
         <v>1473</v>
@@ -7893,7 +7893,7 @@
         <v>24</v>
       </c>
       <c r="BA25" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB25">
         <v>1469</v>
@@ -8025,7 +8025,7 @@
         <v>22</v>
       </c>
       <c r="BA26" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB26">
         <v>2232</v>
@@ -8124,7 +8124,7 @@
         <v>10</v>
       </c>
       <c r="BA27" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB27">
         <v>4515</v>
@@ -8232,7 +8232,7 @@
         <v>45</v>
       </c>
       <c r="BA28" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB28">
         <v>895</v>
@@ -8343,7 +8343,7 @@
         <v>33</v>
       </c>
       <c r="BA29" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB29">
         <v>1223</v>
@@ -8493,7 +8493,7 @@
         <v>34</v>
       </c>
       <c r="BA30" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB30">
         <v>1224</v>
@@ -8625,7 +8625,7 @@
         <v>33</v>
       </c>
       <c r="BA31" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB31">
         <v>1393</v>
@@ -8736,7 +8736,7 @@
         <v>38</v>
       </c>
       <c r="BA32" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB32">
         <v>1568</v>
@@ -8847,7 +8847,7 @@
         <v>27</v>
       </c>
       <c r="BA33" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB33">
         <v>1387</v>
@@ -8958,7 +8958,7 @@
         <v>33</v>
       </c>
       <c r="BA34" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB34">
         <v>2073</v>
@@ -9069,7 +9069,7 @@
         <v>36</v>
       </c>
       <c r="BA35" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB35">
         <v>2416</v>
@@ -9180,7 +9180,7 @@
         <v>30</v>
       </c>
       <c r="BA36" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB36">
         <v>2835</v>
@@ -9291,7 +9291,7 @@
         <v>29</v>
       </c>
       <c r="BA37" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB37">
         <v>3174</v>
@@ -9429,7 +9429,7 @@
         <v>31</v>
       </c>
       <c r="BA38" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB38">
         <v>3516</v>
@@ -9558,7 +9558,7 @@
         <v>32</v>
       </c>
       <c r="BA39" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB39">
         <v>3432</v>
@@ -9669,7 +9669,7 @@
         <v>29</v>
       </c>
       <c r="BA40" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB40">
         <v>3004</v>
@@ -9774,7 +9774,7 @@
         <v>29</v>
       </c>
       <c r="BA41" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB41">
         <v>3259</v>
@@ -9885,7 +9885,7 @@
         <v>25</v>
       </c>
       <c r="BA42" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB42">
         <v>4275</v>
@@ -10014,7 +10014,7 @@
         <v>16</v>
       </c>
       <c r="BA43" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB43">
         <v>4436</v>
@@ -10125,7 +10125,7 @@
         <v>23</v>
       </c>
       <c r="BA44" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB44">
         <v>4613</v>
@@ -10236,7 +10236,7 @@
         <v>25</v>
       </c>
       <c r="BA45" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB45">
         <v>4360</v>
@@ -10365,7 +10365,7 @@
         <v>7</v>
       </c>
       <c r="BA46" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB46">
         <v>8337</v>
@@ -10494,7 +10494,7 @@
         <v>6</v>
       </c>
       <c r="BA47" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB47">
         <v>8166</v>
@@ -10629,7 +10629,7 @@
         <v>1</v>
       </c>
       <c r="BA48" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB48">
         <v>7906</v>
@@ -10758,7 +10758,7 @@
         <v>1</v>
       </c>
       <c r="BA49" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB49">
         <v>8586</v>
@@ -10863,7 +10863,7 @@
         <v>3</v>
       </c>
       <c r="BA50" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB50">
         <v>9353</v>
@@ -10968,7 +10968,7 @@
         <v>3</v>
       </c>
       <c r="BA51" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB51">
         <v>9438</v>
@@ -11073,7 +11073,7 @@
         <v>2</v>
       </c>
       <c r="BA52" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB52">
         <v>9522</v>
@@ -11205,7 +11205,7 @@
         <v>33</v>
       </c>
       <c r="BA53" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB53">
         <v>3518</v>
@@ -11316,7 +11316,7 @@
         <v>34</v>
       </c>
       <c r="BA54" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB54">
         <v>3604</v>
@@ -11424,7 +11424,7 @@
         <v>39</v>
       </c>
       <c r="BA55" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB55">
         <v>4289</v>
@@ -11535,7 +11535,7 @@
         <v>38</v>
       </c>
       <c r="BA56" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB56">
         <v>4543</v>
@@ -11664,7 +11664,7 @@
         <v>12</v>
       </c>
       <c r="BA57" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB57">
         <v>8342</v>
@@ -11763,7 +11763,7 @@
         <v>7</v>
       </c>
       <c r="BA58" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB58">
         <v>9102</v>
@@ -11895,7 +11895,7 @@
         <v>42</v>
       </c>
       <c r="BA59" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB59">
         <v>4292</v>
@@ -12027,7 +12027,7 @@
         <v>46</v>
       </c>
       <c r="BA60" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB60">
         <v>5061</v>
@@ -12159,7 +12159,7 @@
         <v>43</v>
       </c>
       <c r="BA61" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB61">
         <v>4803</v>
@@ -12291,7 +12291,7 @@
         <v>43</v>
       </c>
       <c r="BA62" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB62">
         <v>4378</v>
@@ -12423,7 +12423,7 @@
         <v>38</v>
       </c>
       <c r="BA63" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB63">
         <v>4968</v>
@@ -12534,7 +12534,7 @@
         <v>41</v>
       </c>
       <c r="BA64" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB64">
         <v>5311</v>
@@ -12645,7 +12645,7 @@
         <v>44</v>
       </c>
       <c r="BA65" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB65">
         <v>5229</v>
@@ -12756,7 +12756,7 @@
         <v>37</v>
       </c>
       <c r="BA66" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB66">
         <v>5052</v>
@@ -12888,7 +12888,7 @@
         <v>34</v>
       </c>
       <c r="BA67" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB67">
         <v>6919</v>
@@ -13020,7 +13020,7 @@
         <v>27</v>
       </c>
       <c r="BA68" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB68">
         <v>8527</v>
@@ -13152,7 +13152,7 @@
         <v>27</v>
       </c>
       <c r="BA69" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB69">
         <v>8867</v>
@@ -13281,7 +13281,7 @@
         <v>17</v>
       </c>
       <c r="BA70" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB70">
         <v>9792</v>
@@ -13413,7 +13413,7 @@
         <v>23</v>
       </c>
       <c r="BA71" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB71">
         <v>9883</v>
@@ -13545,7 +13545,7 @@
         <v>22</v>
       </c>
       <c r="BA72" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB72">
         <v>9882</v>
@@ -13683,7 +13683,7 @@
         <v>21</v>
       </c>
       <c r="BA73" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB73">
         <v>9796</v>
@@ -13827,7 +13827,7 @@
         <v>23</v>
       </c>
       <c r="BA74" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB74">
         <v>9883</v>
@@ -13959,7 +13959,7 @@
         <v>22</v>
       </c>
       <c r="BA75" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB75">
         <v>10137</v>
@@ -14091,7 +14091,7 @@
         <v>27</v>
       </c>
       <c r="BA76" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB76">
         <v>9887</v>
@@ -14223,7 +14223,7 @@
         <v>34</v>
       </c>
       <c r="BA77" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB77">
         <v>9639</v>
@@ -14355,7 +14355,7 @@
         <v>31</v>
       </c>
       <c r="BA78" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB78">
         <v>9381</v>
@@ -14466,7 +14466,7 @@
         <v>32</v>
       </c>
       <c r="BA79" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB79">
         <v>10232</v>
@@ -14598,7 +14598,7 @@
         <v>24</v>
       </c>
       <c r="BA80" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB80">
         <v>9884</v>
@@ -14730,7 +14730,7 @@
         <v>31</v>
       </c>
       <c r="BA81" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB81">
         <v>9466</v>
@@ -14862,7 +14862,7 @@
         <v>32</v>
       </c>
       <c r="BA82" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB82">
         <v>9637</v>
@@ -14994,7 +14994,7 @@
         <v>33</v>
       </c>
       <c r="BA83" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB83">
         <v>9893</v>
@@ -15126,7 +15126,7 @@
         <v>26</v>
       </c>
       <c r="BA84" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB84">
         <v>10226</v>
@@ -15264,7 +15264,7 @@
         <v>29</v>
       </c>
       <c r="BA85" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB85">
         <v>9549</v>
@@ -15396,7 +15396,7 @@
         <v>22</v>
       </c>
       <c r="BA86" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB86">
         <v>10222</v>
@@ -15507,7 +15507,7 @@
         <v>22</v>
       </c>
       <c r="BA87" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB87">
         <v>10307</v>
@@ -15618,7 +15618,7 @@
         <v>23</v>
       </c>
       <c r="BA88" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB88">
         <v>10223</v>
@@ -15750,7 +15750,7 @@
         <v>41</v>
       </c>
       <c r="BA89" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB89">
         <v>9901</v>
@@ -15882,7 +15882,7 @@
         <v>29</v>
       </c>
       <c r="BA90" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB90">
         <v>10399</v>
@@ -15993,7 +15993,7 @@
         <v>26</v>
       </c>
       <c r="BA91" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB91">
         <v>11756</v>
@@ -16125,7 +16125,7 @@
         <v>22</v>
       </c>
       <c r="BA92" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB92">
         <v>11157</v>
@@ -16236,7 +16236,7 @@
         <v>24</v>
       </c>
       <c r="BA93" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB93">
         <v>11244</v>
@@ -16347,7 +16347,7 @@
         <v>24</v>
       </c>
       <c r="BA94" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB94">
         <v>11329</v>
@@ -16458,7 +16458,7 @@
         <v>22</v>
       </c>
       <c r="BA95" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB95">
         <v>11242</v>
@@ -16590,7 +16590,7 @@
         <v>24</v>
       </c>
       <c r="BA96" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB96">
         <v>11584</v>
@@ -16728,7 +16728,7 @@
         <v>19</v>
       </c>
       <c r="BA97" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB97">
         <v>11494</v>
@@ -16869,7 +16869,7 @@
         <v>22</v>
       </c>
       <c r="BA98" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB98">
         <v>11922</v>
@@ -17016,7 +17016,7 @@
         <v>21</v>
       </c>
       <c r="BA99" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB99">
         <v>11751</v>
@@ -17145,7 +17145,7 @@
         <v>45</v>
       </c>
       <c r="BA100" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB100">
         <v>8120</v>
@@ -17274,7 +17274,7 @@
         <v>44</v>
       </c>
       <c r="BA101" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB101">
         <v>8459</v>
@@ -17403,7 +17403,7 @@
         <v>45</v>
       </c>
       <c r="BA102" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB102">
         <v>8885</v>
@@ -17526,7 +17526,7 @@
         <v>44</v>
       </c>
       <c r="BA103" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB103">
         <v>8544</v>
@@ -17655,7 +17655,7 @@
         <v>46</v>
       </c>
       <c r="BA104" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB104">
         <v>8886</v>
@@ -17784,7 +17784,7 @@
         <v>44</v>
       </c>
       <c r="BA105" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB105">
         <v>8459</v>
@@ -17883,7 +17883,7 @@
         <v>46</v>
       </c>
       <c r="BA106" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB106">
         <v>9226</v>
@@ -18012,7 +18012,7 @@
         <v>49</v>
       </c>
       <c r="BA107" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB107">
         <v>9484</v>
@@ -18141,7 +18141,7 @@
         <v>42</v>
       </c>
       <c r="BA108" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB108">
         <v>9477</v>
@@ -18249,7 +18249,7 @@
         <v>44</v>
       </c>
       <c r="BA109" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB109">
         <v>9564</v>
@@ -18381,7 +18381,7 @@
         <v>34</v>
       </c>
       <c r="BA110" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB110">
         <v>8534</v>
@@ -18513,7 +18513,7 @@
         <v>42</v>
       </c>
       <c r="BA111" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB111">
         <v>10242</v>
@@ -18624,7 +18624,7 @@
         <v>41</v>
       </c>
       <c r="BA112" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB112">
         <v>10156</v>
@@ -18735,7 +18735,7 @@
         <v>41</v>
       </c>
       <c r="BA113" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB113">
         <v>10241</v>
@@ -18843,7 +18843,7 @@
         <v>43</v>
       </c>
       <c r="BA114" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB114">
         <v>10583</v>
@@ -18981,7 +18981,7 @@
         <v>38</v>
       </c>
       <c r="BA115" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB115">
         <v>11088</v>
@@ -19086,7 +19086,7 @@
         <v>53</v>
       </c>
       <c r="BA116" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB116">
         <v>8723</v>
@@ -19215,7 +19215,7 @@
         <v>50</v>
       </c>
       <c r="BA117" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB117">
         <v>9400</v>
@@ -19344,7 +19344,7 @@
         <v>52</v>
       </c>
       <c r="BA118" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB118">
         <v>9402</v>
@@ -19476,7 +19476,7 @@
         <v>50</v>
       </c>
       <c r="BA119" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB119">
         <v>10760</v>
@@ -19608,7 +19608,7 @@
         <v>51</v>
       </c>
       <c r="BA120" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB120">
         <v>10846</v>
@@ -19740,7 +19740,7 @@
         <v>51</v>
       </c>
       <c r="BA121" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB121">
         <v>10761</v>
@@ -19869,7 +19869,7 @@
         <v>51</v>
       </c>
       <c r="BA122" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB122">
         <v>10506</v>
@@ -20001,7 +20001,7 @@
         <v>47</v>
       </c>
       <c r="BA123" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB123">
         <v>10077</v>
@@ -20112,7 +20112,7 @@
         <v>43</v>
       </c>
       <c r="BA124" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB124">
         <v>10668</v>
@@ -20244,7 +20244,7 @@
         <v>44</v>
       </c>
       <c r="BA125" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB125">
         <v>10754</v>
@@ -20352,7 +20352,7 @@
         <v>44</v>
       </c>
       <c r="BA126" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB126">
         <v>10754</v>
@@ -20463,7 +20463,7 @@
         <v>48</v>
       </c>
       <c r="BA127" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB127">
         <v>10928</v>
@@ -20574,7 +20574,7 @@
         <v>47</v>
       </c>
       <c r="BA128" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB128">
         <v>10842</v>
@@ -20707,7 +20707,7 @@
         <v>49</v>
       </c>
       <c r="BA129" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB129">
         <v>11014</v>
@@ -20854,7 +20854,7 @@
         <v>48</v>
       </c>
       <c r="BA130" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB130">
         <v>11013</v>
@@ -20985,7 +20985,7 @@
         <v>49</v>
       </c>
       <c r="BA131" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB131">
         <v>11014</v>
@@ -21132,7 +21132,7 @@
         <v>53</v>
       </c>
       <c r="BA132" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB132">
         <v>10933</v>
@@ -21265,7 +21265,7 @@
         <v>47</v>
       </c>
       <c r="BA133" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB133">
         <v>11437</v>
@@ -21412,7 +21412,7 @@
         <v>48</v>
       </c>
       <c r="BA134" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB134">
         <v>11608</v>
@@ -21559,7 +21559,7 @@
         <v>43</v>
       </c>
       <c r="BA135" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB135">
         <v>11773</v>
@@ -21706,7 +21706,7 @@
         <v>43</v>
       </c>
       <c r="BA136" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB136">
         <v>11858</v>
@@ -21853,7 +21853,7 @@
         <v>43</v>
       </c>
       <c r="BA137" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB137">
         <v>12283</v>
@@ -21986,7 +21986,7 @@
         <v>41</v>
       </c>
       <c r="BA138" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB138">
         <v>12536</v>
@@ -22118,7 +22118,7 @@
         <v>40</v>
       </c>
       <c r="BA139" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB139">
         <v>11855</v>
@@ -22251,7 +22251,7 @@
         <v>46</v>
       </c>
       <c r="BA140" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB140">
         <v>12201</v>
@@ -22398,7 +22398,7 @@
         <v>31</v>
       </c>
       <c r="BA141" s="6" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB141">
         <v>14056</v>
@@ -22529,7 +22529,7 @@
         <v>31</v>
       </c>
       <c r="BA142" s="6" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB142">
         <v>14056</v>
@@ -22676,7 +22676,7 @@
         <v>31</v>
       </c>
       <c r="BA143" s="6" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB143">
         <v>14396</v>
@@ -22808,7 +22808,7 @@
         <v>28</v>
       </c>
       <c r="BA144" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB144">
         <v>14903</v>
@@ -22959,7 +22959,7 @@
         <v>30</v>
       </c>
       <c r="BA145" s="6" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB145">
         <v>14650</v>
@@ -23106,7 +23106,7 @@
         <v>30</v>
       </c>
       <c r="BA146" s="6" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB146">
         <v>14905</v>
@@ -23233,7 +23233,7 @@
         <v>62</v>
       </c>
       <c r="BA147" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB147">
         <v>10007</v>
@@ -23382,7 +23382,7 @@
         <v>62</v>
       </c>
       <c r="BA148" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB148">
         <v>10007</v>
@@ -23529,7 +23529,7 @@
         <v>59</v>
       </c>
       <c r="BA149" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB149">
         <v>11194</v>
@@ -23676,7 +23676,7 @@
         <v>58</v>
       </c>
       <c r="BA150" s="6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB150">
         <v>11448</v>
@@ -23823,7 +23823,7 @@
         <v>54</v>
       </c>
       <c r="BA151" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB151">
         <v>10934</v>
@@ -23970,7 +23970,7 @@
         <v>55</v>
       </c>
       <c r="BA152" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB152">
         <v>10765</v>
@@ -24117,7 +24117,7 @@
         <v>54</v>
       </c>
       <c r="BA153" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB153">
         <v>10764</v>
@@ -24264,7 +24264,7 @@
         <v>62</v>
       </c>
       <c r="BA154" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB154">
         <v>11027</v>
@@ -24409,7 +24409,7 @@
         <v>62</v>
       </c>
       <c r="BA155" s="6" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB155">
         <v>11197</v>
@@ -24556,7 +24556,7 @@
         <v>57</v>
       </c>
       <c r="BA156" s="6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB156">
         <v>12042</v>
@@ -24689,7 +24689,7 @@
         <v>55</v>
       </c>
       <c r="BA157" s="6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB157">
         <v>11360</v>
@@ -24836,7 +24836,7 @@
         <v>47</v>
       </c>
       <c r="BA158" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB158">
         <v>12202</v>
@@ -24983,7 +24983,7 @@
         <v>48</v>
       </c>
       <c r="BA159" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB159">
         <v>12883</v>
@@ -25114,7 +25114,7 @@
         <v>45</v>
       </c>
       <c r="BA160" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB160">
         <v>13730</v>
@@ -25261,7 +25261,7 @@
         <v>51</v>
       </c>
       <c r="BA161" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB161">
         <v>13141</v>
@@ -25406,7 +25406,7 @@
         <v>77</v>
       </c>
       <c r="BA162" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB162">
         <v>9937</v>
@@ -25551,7 +25551,7 @@
         <v>75</v>
       </c>
       <c r="BA163" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB163">
         <v>10020</v>
@@ -25696,7 +25696,7 @@
         <v>79</v>
       </c>
       <c r="BA164" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB164">
         <v>9939</v>
@@ -25841,7 +25841,7 @@
         <v>71</v>
       </c>
       <c r="BA165" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB165">
         <v>10101</v>
@@ -25986,7 +25986,7 @@
         <v>71</v>
       </c>
       <c r="BA166" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB166">
         <v>10016</v>
@@ -26133,7 +26133,7 @@
         <v>60</v>
       </c>
       <c r="BA167" s="6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB167">
         <v>11960</v>
@@ -26280,7 +26280,7 @@
         <v>62</v>
       </c>
       <c r="BA168" s="6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB168">
         <v>13322</v>
@@ -26413,7 +26413,7 @@
         <v>60</v>
       </c>
       <c r="BA169" s="6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB169">
         <v>12980</v>
@@ -26560,7 +26560,7 @@
         <v>55</v>
       </c>
       <c r="BA170" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB170">
         <v>14420</v>
@@ -26705,7 +26705,7 @@
         <v>78</v>
       </c>
       <c r="BA171" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB171">
         <v>11553</v>
@@ -26852,7 +26852,7 @@
         <v>71</v>
       </c>
       <c r="BA172" s="6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB172">
         <v>16306</v>
@@ -26979,7 +26979,7 @@
         <v>48</v>
       </c>
       <c r="BA173" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB173">
         <v>3363</v>
@@ -27106,7 +27106,7 @@
         <v>36</v>
       </c>
       <c r="BA174" s="6" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB174">
         <v>1991</v>
@@ -27233,7 +27233,7 @@
         <v>59</v>
       </c>
       <c r="BA175" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB175">
         <v>1504</v>
@@ -27360,7 +27360,7 @@
         <v>38</v>
       </c>
       <c r="BA176" s="6" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB176">
         <v>6838</v>
@@ -27487,7 +27487,7 @@
         <v>45</v>
       </c>
       <c r="BA177" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB177">
         <v>8120</v>
@@ -27618,7 +27618,7 @@
         <v>44</v>
       </c>
       <c r="BA178" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB178">
         <v>8459</v>
@@ -27749,7 +27749,7 @@
         <v>46</v>
       </c>
       <c r="BA179" s="6" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB179">
         <v>8886</v>
@@ -27876,7 +27876,7 @@
         <v>41</v>
       </c>
       <c r="BA180" s="6" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB180">
         <v>13641</v>
@@ -28005,7 +28005,7 @@
         <v>57</v>
       </c>
       <c r="BA181" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB181">
         <v>11787</v>
@@ -28134,7 +28134,7 @@
         <v>36</v>
       </c>
       <c r="BA182" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB182">
         <v>12191</v>
@@ -28263,7 +28263,7 @@
         <v>36</v>
       </c>
       <c r="BA183" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB183">
         <v>12191</v>
@@ -28392,7 +28392,7 @@
         <v>36</v>
       </c>
       <c r="BA184" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB184">
         <v>12191</v>
@@ -28527,7 +28527,7 @@
         <v>36</v>
       </c>
       <c r="BA185" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB185">
         <v>12191</v>
@@ -28656,7 +28656,7 @@
         <v>36</v>
       </c>
       <c r="BA186" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB186">
         <v>12191</v>
@@ -28785,7 +28785,7 @@
         <v>46</v>
       </c>
       <c r="BA187" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB187">
         <v>13306</v>
@@ -28914,7 +28914,7 @@
         <v>46</v>
       </c>
       <c r="BA188" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB188">
         <v>13306</v>
@@ -29043,7 +29043,7 @@
         <v>46</v>
       </c>
       <c r="BA189" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB189">
         <v>13306</v>
@@ -29172,7 +29172,7 @@
         <v>46</v>
       </c>
       <c r="BA190" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB190">
         <v>13306</v>
@@ -29301,7 +29301,7 @@
         <v>55</v>
       </c>
       <c r="BA191" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB191">
         <v>11955</v>
@@ -29403,7 +29403,7 @@
         <v>32</v>
       </c>
       <c r="BA192" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB192">
         <v>9807</v>
@@ -29505,7 +29505,7 @@
         <v>32</v>
       </c>
       <c r="BA193" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB193">
         <v>9807</v>
@@ -29634,7 +29634,7 @@
         <v>32</v>
       </c>
       <c r="BA194" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB194">
         <v>9807</v>
@@ -29763,7 +29763,7 @@
         <v>20</v>
       </c>
       <c r="BA195" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB195">
         <v>11070</v>
@@ -29892,7 +29892,7 @@
         <v>47</v>
       </c>
       <c r="BA196" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB196">
         <v>10162</v>
@@ -30021,7 +30021,7 @@
         <v>47</v>
       </c>
       <c r="BA197" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB197">
         <v>10162</v>
@@ -30150,7 +30150,7 @@
         <v>48</v>
       </c>
       <c r="BA198" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB198">
         <v>10248</v>
@@ -30252,7 +30252,7 @@
         <v>47</v>
       </c>
       <c r="BA199" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB199">
         <v>10247</v>
@@ -30354,7 +30354,7 @@
         <v>46</v>
       </c>
       <c r="BA200" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB200">
         <v>13306</v>
@@ -30456,7 +30456,7 @@
         <v>36</v>
       </c>
       <c r="BA201" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB201">
         <v>12191</v>
@@ -30558,7 +30558,7 @@
         <v>39</v>
       </c>
       <c r="BA202" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB202">
         <v>9899</v>
@@ -30687,7 +30687,7 @@
         <v>40</v>
       </c>
       <c r="BA203" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB203">
         <v>10495</v>
@@ -30816,7 +30816,7 @@
         <v>46</v>
       </c>
       <c r="BA204" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB204">
         <v>11691</v>
@@ -30945,7 +30945,7 @@
         <v>46</v>
       </c>
       <c r="BA205" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB205">
         <v>11691</v>
@@ -31074,7 +31074,7 @@
         <v>46</v>
       </c>
       <c r="BA206" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB206">
         <v>11606</v>
@@ -31203,7 +31203,7 @@
         <v>36</v>
       </c>
       <c r="BA207" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB207">
         <v>9811</v>
@@ -31332,7 +31332,7 @@
         <v>36</v>
       </c>
       <c r="BA208" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB208">
         <v>9811</v>
@@ -31431,7 +31431,7 @@
         <v>51</v>
       </c>
       <c r="BA209" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB209">
         <v>10506</v>
@@ -31560,7 +31560,7 @@
         <v>36</v>
       </c>
       <c r="BA210" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="BB210">
         <v>1396</v>
@@ -31689,7 +31689,7 @@
         <v>25</v>
       </c>
       <c r="BA211" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB211">
         <v>10395</v>
@@ -31788,7 +31788,7 @@
         <v>50</v>
       </c>
       <c r="BA212" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="BB212">
         <v>10505</v>
@@ -31917,7 +31917,7 @@
         <v>29</v>
       </c>
       <c r="BA213" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB213">
         <v>10569</v>
@@ -32046,7 +32046,7 @@
         <v>29</v>
       </c>
       <c r="BA214" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB214">
         <v>10569</v>
@@ -32175,7 +32175,7 @@
         <v>34</v>
       </c>
       <c r="BA215" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB215">
         <v>5559</v>
@@ -32304,7 +32304,7 @@
         <v>36</v>
       </c>
       <c r="BA216" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="BB216">
         <v>7176</v>
@@ -32433,7 +32433,7 @@
         <v>38</v>
       </c>
       <c r="BA217" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB217">
         <v>8453</v>
@@ -32562,7 +32562,7 @@
         <v>37</v>
       </c>
       <c r="BA218" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB218">
         <v>11427</v>
@@ -32691,7 +32691,7 @@
         <v>29</v>
       </c>
       <c r="BA219" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB219">
         <v>10569</v>
@@ -32820,7 +32820,7 @@
         <v>29</v>
       </c>
       <c r="BA220" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="BB220">
         <v>10569</v>
@@ -32949,7 +32949,7 @@
         <v>58</v>
       </c>
       <c r="BA221" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB221">
         <v>11703</v>
@@ -33078,7 +33078,7 @@
         <v>58</v>
       </c>
       <c r="BA222" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB222">
         <v>11703</v>
@@ -33207,7 +33207,7 @@
         <v>61</v>
       </c>
       <c r="BA223" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB223">
         <v>13661</v>
@@ -33336,7 +33336,7 @@
         <v>61</v>
       </c>
       <c r="BA224" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="BB224">
         <v>13661</v>
@@ -33465,7 +33465,7 @@
         <v>25</v>
       </c>
       <c r="BA225" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB225">
         <v>11500</v>
@@ -33594,7 +33594,7 @@
         <v>25</v>
       </c>
       <c r="BA226" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB226">
         <v>11500</v>
@@ -33723,7 +33723,7 @@
         <v>25</v>
       </c>
       <c r="BA227" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB227">
         <v>11500</v>
@@ -36519,7 +36519,7 @@
         <v>22</v>
       </c>
       <c r="BA252" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB252">
         <v>14472</v>
@@ -36648,7 +36648,7 @@
         <v>22</v>
       </c>
       <c r="BA253" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="BB253">
         <v>14472</v>
@@ -36777,7 +36777,7 @@
         <v>48</v>
       </c>
       <c r="BA254" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB254">
         <v>13053</v>
@@ -36879,7 +36879,7 @@
         <v>7</v>
       </c>
       <c r="BA255" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB255">
         <v>4172</v>
@@ -36981,7 +36981,7 @@
         <v>53</v>
       </c>
       <c r="BA256" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="BB256">
         <v>8128</v>
@@ -37110,7 +37110,7 @@
         <v>19</v>
       </c>
       <c r="BA257" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="BB257">
         <v>18379</v>
@@ -37239,7 +37239,7 @@
         <v>48</v>
       </c>
       <c r="BA258" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB258">
         <v>13308</v>
@@ -37368,7 +37368,7 @@
         <v>48</v>
       </c>
       <c r="BA259" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB259">
         <v>13478</v>
@@ -37497,7 +37497,7 @@
         <v>50</v>
       </c>
       <c r="BA260" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="BB260">
         <v>13310</v>

</xml_diff>